<commit_message>
Deploying to gh-pages from  @ 8d8cc2669ec3a9ad5ffa6da459d1f6ba6700f055 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_4-2-1.xlsx
+++ b/assets/excel/2021_4-2-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A2A6765-A084-4A5A-8108-E39E2701A6B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37A97AC4-F153-4599-BEA8-F68F82067F10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{28D2177B-DBE4-483C-A493-BE8559B9A136}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{28D2177B-DBE4-483C-A493-BE8559B9A136}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -273,53 +273,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -954,461 +954,461 @@
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:12" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="9"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="2:12" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11" t="s">
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="2:12" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:12" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="2:12" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:12" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
+      <c r="B12" s="9">
         <v>2020</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="11">
         <v>25</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="11">
         <v>31.4</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="11">
         <v>18.100000000000001</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="11">
         <v>26.5</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="11">
         <v>33.700000000000003</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="11">
         <v>19</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="11">
         <v>12.1</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="11">
         <v>14.2</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="11">
         <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="13" spans="2:12" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
+      <c r="B13" s="9">
         <v>2019</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="11">
         <v>26.3</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="11">
         <v>32.5</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="11">
         <v>19.399999999999999</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="11">
         <v>28.1</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="11">
         <v>35.200000000000003</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="11">
         <v>20.6</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="11">
         <v>12.6</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="11">
         <v>14.9</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="11">
         <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="14" spans="2:12" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
+      <c r="B14" s="9">
         <v>2018</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="11">
         <v>26.2</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="11">
         <v>32.1</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="11">
         <v>19.7</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="11">
         <v>28.3</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="11">
         <v>35.200000000000003</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="11">
         <v>21</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="11">
         <v>11.5</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="11">
         <v>13.5</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="11">
         <v>8.6</v>
       </c>
     </row>
     <row r="15" spans="2:12" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
+      <c r="B15" s="9">
         <v>2017</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="11">
         <v>26.1</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="11">
         <v>31.4</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="11">
         <v>20.399999999999999</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="11">
         <v>28.5</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="11">
         <v>34.9</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="11">
         <v>21.7</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="11">
         <v>9.3000000000000007</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="11">
         <v>9.9</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="11">
         <v>8.5</v>
       </c>
     </row>
     <row r="16" spans="2:12" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16">
+      <c r="B16" s="9">
         <v>2016</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="11">
         <v>26.4</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="11">
         <v>31.4</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="11">
         <v>20.9</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="11">
         <v>28.9</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="11">
         <v>35.200000000000003</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="11">
         <v>22.3</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="11">
         <v>7.4</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="11">
         <v>7.1</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="11">
         <v>7.8</v>
       </c>
     </row>
     <row r="17" spans="2:11" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="16">
+      <c r="B17" s="9">
         <v>2015</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="11">
         <v>26.5</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="11">
         <v>31.4</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="11">
         <v>21</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="11">
         <v>29</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="11">
         <v>35.200000000000003</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="11">
         <v>22.5</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="11">
         <v>6</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="11">
         <v>6.2</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="11">
         <v>5.7</v>
       </c>
     </row>
     <row r="18" spans="2:11" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16">
+      <c r="B18" s="9">
         <v>2014</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="11">
         <v>27.8</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="11">
         <v>33.5</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="11">
         <v>21.6</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="11">
         <v>29.5</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="11">
         <v>35.799999999999997</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="11">
         <v>22.8</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="11">
         <v>8.1999999999999993</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="11">
         <v>9.4</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="11">
         <v>6.8</v>
       </c>
     </row>
     <row r="19" spans="2:11" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="16">
+      <c r="B19" s="9">
         <v>2013</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="11">
         <v>29</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="11">
         <v>34.799999999999997</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="11">
         <v>22.9</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="11">
         <v>30.5</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="11">
         <v>36.5</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="11">
         <v>23.9</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="11">
         <v>9.8000000000000007</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="11">
         <v>11.2</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19" s="11">
         <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="20" spans="2:11" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="16">
+      <c r="B20" s="9">
         <v>2012</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="11">
         <v>29.5</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="11">
         <v>35.200000000000003</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="11">
         <v>23.4</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="11">
         <v>30.8</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="11">
         <v>36.799999999999997</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="11">
         <v>24.4</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="11">
         <v>10.199999999999999</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="11">
         <v>11.2</v>
       </c>
-      <c r="K20" s="18">
+      <c r="K20" s="11">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="2:11" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="16">
+      <c r="B21" s="9">
         <v>2011</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="11">
         <v>29.7</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="11">
         <v>35</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="11">
         <v>24.1</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="11">
         <v>30.9</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="11">
         <v>36.4</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="11">
         <v>25</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="11">
         <v>11.2</v>
       </c>
-      <c r="J21" s="18">
+      <c r="J21" s="11">
         <v>12.5</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K21" s="11">
         <v>9.6</v>
       </c>
     </row>
     <row r="22" spans="2:11" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
     </row>
     <row r="23" spans="2:11" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
     </row>
     <row r="24" spans="2:11" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="21"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1513,7 +1513,7 @@
       <c r="K31" s="5"/>
     </row>
     <row r="32" spans="2:11" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C32" s="5"/>

</xml_diff>